<commit_message>
Completed binding (billing plan), added fields and methods  for tenant, updated logs and excel data
</commit_message>
<xml_diff>
--- a/CucumberTest/src/TestData/HomeownersTestData.xlsx
+++ b/CucumberTest/src/TestData/HomeownersTestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KatarinaGigic\Desktop\Sandbox\Sandbox-Automation\CucumberTest\src\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adragutinovic\Desktop\Projekti\Sandbox-Automation\CucumberTest\src\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{841AC8C7-FAC4-4093-A1AC-6AE8EFE472EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56E6B53E-CA22-4415-9DA3-474CCEB3F265}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{B28A2263-319C-43F1-A09A-167E32921814}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{B28A2263-319C-43F1-A09A-167E32921814}"/>
   </bookViews>
   <sheets>
     <sheet name="HomePage" sheetId="1" r:id="rId1"/>
@@ -778,13 +778,13 @@
     <t>1000000</t>
   </si>
   <si>
-    <t>1,00</t>
-  </si>
-  <si>
     <t>2018</t>
   </si>
   <si>
     <t>The floor on which the risk is located</t>
+  </si>
+  <si>
+    <t>Bronze</t>
   </si>
 </sst>
 </file>
@@ -1008,7 +1008,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1326,23 +1326,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{233E3F76-9812-476D-B6C2-B4C4C2D25A3F}">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" customWidth="1"/>
+    <col min="6" max="7" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.44140625" customWidth="1"/>
     <col min="9" max="9" width="19" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="16" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="21" width="13.5703125" customWidth="1"/>
+    <col min="17" max="17" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="21" width="13.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1371,7 +1371,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -1394,7 +1394,7 @@
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
@@ -1419,7 +1419,7 @@
       </c>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -1442,7 +1442,7 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -1467,7 +1467,7 @@
       </c>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -1478,7 +1478,7 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1489,7 +1489,7 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -1500,7 +1500,7 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1511,7 +1511,7 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -1522,7 +1522,7 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1533,7 +1533,7 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1544,7 +1544,7 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1555,7 +1555,7 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1566,7 +1566,7 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1577,7 +1577,7 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1588,7 +1588,7 @@
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1599,7 +1599,7 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1610,7 +1610,7 @@
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1621,7 +1621,7 @@
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1632,7 +1632,7 @@
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1654,25 +1654,25 @@
   <dimension ref="A1:Q21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" customWidth="1"/>
-    <col min="7" max="11" width="18.140625" customWidth="1"/>
-    <col min="12" max="13" width="17.140625" customWidth="1"/>
-    <col min="14" max="14" width="11.7109375" customWidth="1"/>
-    <col min="16" max="16" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.88671875" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5546875" customWidth="1"/>
+    <col min="7" max="11" width="18.109375" customWidth="1"/>
+    <col min="12" max="13" width="17.109375" customWidth="1"/>
+    <col min="14" max="14" width="11.6640625" customWidth="1"/>
+    <col min="16" max="16" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
@@ -1725,7 +1725,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>38</v>
       </c>
@@ -1768,7 +1768,7 @@
       </c>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>87</v>
       </c>
@@ -1811,7 +1811,7 @@
       </c>
       <c r="Q3" s="1"/>
     </row>
-    <row r="4" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>88</v>
       </c>
@@ -1854,7 +1854,7 @@
       </c>
       <c r="Q4" s="1"/>
     </row>
-    <row r="5" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>89</v>
       </c>
@@ -1897,7 +1897,7 @@
       </c>
       <c r="Q5" s="1"/>
     </row>
-    <row r="6" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>90</v>
       </c>
@@ -1940,7 +1940,7 @@
       </c>
       <c r="Q6" s="1"/>
     </row>
-    <row r="7" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>91</v>
       </c>
@@ -1982,7 +1982,7 @@
       </c>
       <c r="Q7" s="1"/>
     </row>
-    <row r="8" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>92</v>
       </c>
@@ -2025,7 +2025,7 @@
       </c>
       <c r="Q8" s="1"/>
     </row>
-    <row r="9" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>93</v>
       </c>
@@ -2038,7 +2038,7 @@
       <c r="D9" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="E9" s="11" t="s">
         <v>226</v>
       </c>
       <c r="F9" s="9" t="s">
@@ -2068,7 +2068,7 @@
       </c>
       <c r="Q9" s="1"/>
     </row>
-    <row r="10" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>94</v>
       </c>
@@ -2081,7 +2081,7 @@
       <c r="D10" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="E10" s="18" t="s">
+      <c r="E10" s="12" t="s">
         <v>227</v>
       </c>
       <c r="F10" s="9" t="s">
@@ -2111,7 +2111,7 @@
       </c>
       <c r="Q10" s="1"/>
     </row>
-    <row r="11" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>95</v>
       </c>
@@ -2124,7 +2124,7 @@
       <c r="D11" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="E11" s="18" t="s">
+      <c r="E11" s="12" t="s">
         <v>228</v>
       </c>
       <c r="F11" s="9" t="s">
@@ -2154,7 +2154,7 @@
       </c>
       <c r="Q11" s="1"/>
     </row>
-    <row r="12" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>96</v>
       </c>
@@ -2167,7 +2167,7 @@
       <c r="D12" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="E12" s="18" t="s">
+      <c r="E12" s="12" t="s">
         <v>229</v>
       </c>
       <c r="F12" s="9" t="s">
@@ -2197,7 +2197,7 @@
       </c>
       <c r="Q12" s="1"/>
     </row>
-    <row r="13" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>97</v>
       </c>
@@ -2210,7 +2210,7 @@
       <c r="D13" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="E13" s="18" t="s">
+      <c r="E13" s="12" t="s">
         <v>230</v>
       </c>
       <c r="F13" s="9" t="s">
@@ -2240,7 +2240,7 @@
       </c>
       <c r="Q13" s="1"/>
     </row>
-    <row r="14" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>98</v>
       </c>
@@ -2253,7 +2253,7 @@
       <c r="D14" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="E14" s="18" t="s">
+      <c r="E14" s="12" t="s">
         <v>231</v>
       </c>
       <c r="F14" s="9" t="s">
@@ -2283,7 +2283,7 @@
       </c>
       <c r="Q14" s="1"/>
     </row>
-    <row r="15" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>99</v>
       </c>
@@ -2296,7 +2296,7 @@
       <c r="D15" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="E15" s="18" t="s">
+      <c r="E15" s="12" t="s">
         <v>232</v>
       </c>
       <c r="F15" s="9" t="s">
@@ -2326,7 +2326,7 @@
       </c>
       <c r="Q15" s="1"/>
     </row>
-    <row r="16" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>100</v>
       </c>
@@ -2339,7 +2339,7 @@
       <c r="D16" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="E16" s="18" t="s">
+      <c r="E16" s="11" t="s">
         <v>233</v>
       </c>
       <c r="F16" s="9" t="s">
@@ -2369,7 +2369,7 @@
       </c>
       <c r="Q16" s="1"/>
     </row>
-    <row r="17" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>101</v>
       </c>
@@ -2382,7 +2382,7 @@
       <c r="D17" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="E17" s="18" t="s">
+      <c r="E17" s="12" t="s">
         <v>234</v>
       </c>
       <c r="F17" s="9" t="s">
@@ -2412,7 +2412,7 @@
       </c>
       <c r="Q17" s="1"/>
     </row>
-    <row r="18" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>102</v>
       </c>
@@ -2425,7 +2425,7 @@
       <c r="D18" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E18" s="18" t="s">
+      <c r="E18" s="12" t="s">
         <v>235</v>
       </c>
       <c r="F18" s="9" t="s">
@@ -2455,7 +2455,7 @@
       </c>
       <c r="Q18" s="1"/>
     </row>
-    <row r="19" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>103</v>
       </c>
@@ -2468,7 +2468,7 @@
       <c r="D19" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="E19" s="18" t="s">
+      <c r="E19" s="12" t="s">
         <v>236</v>
       </c>
       <c r="F19" s="9" t="s">
@@ -2498,7 +2498,7 @@
       </c>
       <c r="Q19" s="1"/>
     </row>
-    <row r="20" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>104</v>
       </c>
@@ -2511,7 +2511,7 @@
       <c r="D20" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="E20" s="18" t="s">
+      <c r="E20" s="12" t="s">
         <v>237</v>
       </c>
       <c r="F20" s="9" t="s">
@@ -2541,20 +2541,20 @@
       </c>
       <c r="Q20" s="1"/>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>105</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="1" t="s">
         <v>142</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="E21" s="18" t="s">
+      <c r="E21" s="12" t="s">
         <v>238</v>
       </c>
       <c r="F21" s="9" t="s">
@@ -2618,37 +2618,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{218C4EAF-DA0D-41F4-8693-75C9583F20AE}">
   <dimension ref="A1:AC9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X16" sqref="X16"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.7109375" customWidth="1"/>
-    <col min="4" max="4" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="54.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="54.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.6640625" customWidth="1"/>
+    <col min="4" max="4" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="54.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="54.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="18.140625" customWidth="1"/>
-    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="29.140625" customWidth="1"/>
-    <col min="14" max="14" width="29.85546875" customWidth="1"/>
-    <col min="15" max="15" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.5703125" customWidth="1"/>
-    <col min="25" max="25" width="16.42578125" customWidth="1"/>
-    <col min="26" max="26" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="61.85546875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="42.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="18.109375" customWidth="1"/>
+    <col min="12" max="12" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="29.109375" customWidth="1"/>
+    <col min="14" max="14" width="29.88671875" customWidth="1"/>
+    <col min="15" max="15" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.5546875" customWidth="1"/>
+    <col min="25" max="25" width="16.44140625" customWidth="1"/>
+    <col min="26" max="26" width="31.5546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="61.88671875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="42.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
         <v>47</v>
       </c>
@@ -2722,7 +2722,7 @@
         <v>243</v>
       </c>
       <c r="Y1" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="Z1" s="15" t="s">
         <v>71</v>
@@ -2737,7 +2737,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>49</v>
       </c>
@@ -2814,7 +2814,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>49</v>
       </c>
@@ -2899,7 +2899,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>49</v>
       </c>
@@ -2922,16 +2922,16 @@
         <v>50</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>50</v>
+        <v>248</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>240</v>
       </c>
       <c r="J4" s="10"/>
-      <c r="K4" s="1">
+      <c r="K4" s="18">
         <v>500000</v>
       </c>
-      <c r="L4" s="1">
+      <c r="L4" s="18">
         <v>100000</v>
       </c>
       <c r="M4" s="1" t="s">
@@ -2941,7 +2941,7 @@
         <v>50</v>
       </c>
       <c r="O4" s="10" t="s">
-        <v>246</v>
+        <v>76</v>
       </c>
       <c r="P4" s="10" t="s">
         <v>77</v>
@@ -2953,7 +2953,7 @@
         <v>76</v>
       </c>
       <c r="S4" s="10" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="T4" s="1" t="s">
         <v>86</v>
@@ -2986,7 +2986,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>49</v>
       </c>
@@ -3027,7 +3027,7 @@
       <c r="AB5" s="1"/>
       <c r="AC5" s="1"/>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -3058,7 +3058,7 @@
       <c r="AB6" s="1"/>
       <c r="AC6" s="1"/>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -3089,7 +3089,7 @@
       <c r="AB7" s="1"/>
       <c r="AC7" s="1"/>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -3120,7 +3120,7 @@
       <c r="AB8" s="1"/>
       <c r="AC8" s="1"/>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>

</xml_diff>

<commit_message>
implemented Regression method for home
</commit_message>
<xml_diff>
--- a/CucumberTest/src/TestData/HomeownersTestData.xlsx
+++ b/CucumberTest/src/TestData/HomeownersTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KatarinaGigic\Desktop\Sandbox1\Sandbox-Automation\CucumberTest\src\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3432290C-BA8B-4D31-B0A8-7CAF6B5BEF23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F408F1A2-ABFA-43D6-806A-DD6401FD7C9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{B28A2263-319C-43F1-A09A-167E32921814}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="2" xr2:uid="{B28A2263-319C-43F1-A09A-167E32921814}"/>
   </bookViews>
   <sheets>
     <sheet name="HomePage" sheetId="1" r:id="rId1"/>
@@ -2680,8 +2680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{218C4EAF-DA0D-41F4-8693-75C9583F20AE}">
   <dimension ref="A1:AK19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AK19" sqref="AK19"/>
+    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
+      <selection activeCell="AD1" sqref="AD1:AD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2708,7 +2708,7 @@
     <col min="27" max="27" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="61.85546875" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="13.28515625" customWidth="1"/>
+    <col min="30" max="30" width="24.7109375" customWidth="1"/>
     <col min="31" max="31" width="35" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="25.140625" customWidth="1"/>
     <col min="33" max="33" width="27.85546875" customWidth="1"/>

</xml_diff>